<commit_message>
YF23A-4 modify SFM data, add cockpit texture
</commit_message>
<xml_diff>
--- a/Docs/enginedata_sim.xlsx
+++ b/Docs/enginedata_sim.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChromeDownloads\YF-23A assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Saved Games\DCS\Mods\aircraft\YF-23A Black Widow\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48780BBD-5100-4590-8934-3AE8106A5F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3825AFA6-652C-4E53-9421-9E978DFFB0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-270" yWindow="315" windowWidth="26070" windowHeight="15120" activeTab="3" xr2:uid="{4FF444EB-0F0D-40DE-8406-3D4C9ADBD34C}"/>
+    <workbookView xWindow="-2460" yWindow="720" windowWidth="28800" windowHeight="15120" activeTab="3" xr2:uid="{4FF444EB-0F0D-40DE-8406-3D4C9ADBD34C}"/>
   </bookViews>
   <sheets>
     <sheet name="Pfor" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>kg</t>
   </si>
@@ -236,6 +236,14 @@
   </si>
   <si>
     <t>Pfor-Sim-3-tuned</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pmax-Sim-5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pfor-Sim-5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3575,11 +3583,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sim!$A$2</c:f>
+              <c:f>Sim!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pmax-Sim-1</c:v>
+                  <c:v>Pmax-Sim-5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3589,7 +3597,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:prstDash val="sysDot"/>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3659,60 +3667,60 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sim!$B$2:$R$2</c:f>
+              <c:f>Sim!$B$9:$R$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>116263.1679592</c:v>
+                  <c:v>131440.5005104997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105485.1270224</c:v>
+                  <c:v>123571.59647303399</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98572.590656</c:v>
+                  <c:v>118651.86336651219</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>94813.843403999999</c:v>
+                  <c:v>116258.72013748079</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93937.543748800003</c:v>
+                  <c:v>115902.86240825678</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>93648.409344800006</c:v>
+                  <c:v>116058.55016479229</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>93897.509754400002</c:v>
+                  <c:v>116694.6458557802</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>94622.569875200003</c:v>
+                  <c:v>117780.01192991339</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>95267.562007200002</c:v>
+                  <c:v>118785.31001497118</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>95988.173906399999</c:v>
+                  <c:v>119879.57253233499</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>96824.439567199996</c:v>
+                  <c:v>121133.97102784959</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>97736.324995200004</c:v>
+                  <c:v>122535.16083666909</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>99520.061856800006</c:v>
+                  <c:v>125635.57130253319</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100596.53148400001</c:v>
+                  <c:v>128758.2228764738</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>96188.343878400003</c:v>
+                  <c:v>130159.41268529328</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>94560.2947728</c:v>
+                  <c:v>130159.41268529328</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>94560.2947728</c:v>
+                  <c:v>130159.41268529328</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3729,11 +3737,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sim!$A$3</c:f>
+              <c:f>Sim!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pfor-Sim-1</c:v>
+                  <c:v>Pfor-Sim-5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3743,7 +3751,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:prstDash val="sysDot"/>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3813,60 +3821,60 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sim!$B$3:$R$3</c:f>
+              <c:f>Sim!$B$10:$R$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>156266.02480800002</c:v>
+                  <c:v>156372.7826642562</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>146519.97128240002</c:v>
+                  <c:v>148837.495247938</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>142650.01849039999</c:v>
+                  <c:v>144931.95666970458</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>144073.4494024</c:v>
+                  <c:v>144286.9645354861</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146675.65903840002</c:v>
+                  <c:v>145105.43731270128</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>150518.92250079999</c:v>
+                  <c:v>146653.4184348257</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>155616.5844544</c:v>
+                  <c:v>148917.56323701338</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>161981.98956400002</c:v>
+                  <c:v>151893.42349764908</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>168827.80260640002</c:v>
+                  <c:v>154918.21419605307</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>176460.95087200002</c:v>
+                  <c:v>158245.48396429748</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>185046.01856</c:v>
+                  <c:v>161981.99012114949</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>194623.03966480002</c:v>
+                  <c:v>166154.42199630089</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>216757.3903464</c:v>
+                  <c:v>175762.58068534889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>242690.52227440002</c:v>
+                  <c:v>186900.92761006008</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>303235.26647199999</c:v>
+                  <c:v>192954.95722848337</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>311228.72068720002</c:v>
+                  <c:v>192954.95722848337</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>311228.72068720002</c:v>
+                  <c:v>192954.95722848337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3875,781 +3883,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6BCC-445E-BC8D-BA796343BD74}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sim!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Pmax-Sim-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="lgDashDotDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sim!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sim!$B$4:$R$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>142863.5336185901</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>133798.0579666087</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>129750.17629668569</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>130159.41268529328</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>131929.8048881827</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>134718.83984097579</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>138513.17287882668</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>143312.80400173538</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148432.70708094569</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>154108.63786206848</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160469.59477194748</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>167520.02603219799</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>183609.24361473808</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>201967.05422108117</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>241818.67167255387</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>246636.09568192379</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>246636.09568192379</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6BCC-445E-BC8D-BA796343BD74}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sim!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Pfor-Sim-2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:prstDash val="lgDashDotDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sim!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sim!$B$5:$R$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>156577.40085855999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>147783.2667251119</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>144602.7882701724</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>146528.86822959728</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>149340.14429046688</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>153379.12951715928</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>158654.72035290507</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>165202.50257062668</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>172257.3820524925</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>180130.73431157347</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>188996.03999086638</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>198902.22952813949</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>221917.32816570168</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>249180.47844587537</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>314809.54015801154</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>323781.60315607168</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>323781.60315607168</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-6BCC-445E-BC8D-BA796343BD74}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sim!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Pmax-Sim-3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sim!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sim!$B$6:$R$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>130880.02458697189</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>121605.48251907139</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>116957.09093108289</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>116316.54701847969</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>117375.22376292109</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>119301.30372234598</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>122081.44223190848</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>125688.94996191679</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>129478.83477815239</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>133660.16309653438</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>138317.45112775348</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>143437.35420696379</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>154842.59442859297</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>167217.54696235759</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>189907.92542200288</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>191976.3484731174</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>191976.3484731174</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-6BCC-445E-BC8D-BA796343BD74}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sim!$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Pfor-Sim-3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sim!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sim!$B$7:$R$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>157031.11946332059</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>148312.60509733259</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>145367.88238800399</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>147707.6469576518</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>150799.16098028529</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>155176.21104974049</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>160861.03827409388</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>167884.78020465258</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>175477.89450196968</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>183960.65312234679</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>193519.88137362647</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>204226.75080165357</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>229221.30805802427</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>259064.42687507198</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>332357.77443037007</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>342584.2359239448</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>342584.2359239448</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-6BCC-445E-BC8D-BA796343BD74}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sim!$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PFor-Sim-1-Tuned</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="sysDot"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sim!$B$1:$R$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sim!$B$8:$R$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>156266.02480800002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>146519.97128240002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>142650.01849039999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>144073.4494024</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>146675.65903840002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>150518.92250079999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>155616.5844544</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>159000.98956399999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>164827.80260639999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>171460.95087199999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>179046.01856</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>187623.03966479999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>195100.3903464</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>193266</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>193266</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>190000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>190000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-6BCC-445E-BC8D-BA796343BD74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11603,11 +10836,11 @@
       <sheetName val="SFM_Data_Reference"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
       <sheetData sheetId="5">
         <row r="64">
           <cell r="C64">
@@ -11615,8 +10848,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -13853,13 +13086,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F00D91-73F8-42BA-A576-203C4D4B4B33}">
   <dimension ref="A1:AK46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="20" max="20" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
@@ -14026,55 +13260,55 @@
         <v>5</v>
       </c>
       <c r="U2" s="3">
-        <v>35302</v>
+        <v>35154</v>
       </c>
       <c r="V2" s="3">
-        <v>33342</v>
+        <v>33460</v>
       </c>
       <c r="W2" s="3">
-        <v>32680</v>
+        <v>32582</v>
       </c>
       <c r="X2" s="3">
-        <v>33206</v>
+        <v>32437</v>
       </c>
       <c r="Y2" s="3">
-        <v>33901</v>
+        <v>32621</v>
       </c>
       <c r="Z2" s="3">
-        <v>34885</v>
+        <v>32969</v>
       </c>
       <c r="AA2" s="3">
-        <v>36163</v>
+        <v>33478</v>
       </c>
       <c r="AB2" s="3">
-        <v>37742</v>
+        <v>34147</v>
       </c>
       <c r="AC2" s="3">
-        <v>39449</v>
+        <v>34827</v>
       </c>
       <c r="AD2" s="3">
-        <v>41356</v>
+        <v>35575</v>
       </c>
       <c r="AE2" s="3">
-        <v>43505</v>
+        <v>36415</v>
       </c>
       <c r="AF2" s="3">
-        <v>45912</v>
+        <v>37353</v>
       </c>
       <c r="AG2" s="3">
-        <v>51531</v>
+        <v>39513</v>
       </c>
       <c r="AH2" s="3">
-        <v>58240</v>
+        <v>42017</v>
       </c>
       <c r="AI2" s="3">
-        <v>74717</v>
+        <v>43378</v>
       </c>
       <c r="AJ2" s="3">
-        <v>77016</v>
+        <v>43378</v>
       </c>
       <c r="AK2" s="3">
-        <v>77016</v>
+        <v>43378</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
@@ -14137,71 +13371,71 @@
       </c>
       <c r="U3" s="3" cm="1">
         <f t="array" aca="1" ref="U3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>157031.11946332059</v>
+        <v>156372.7826642562</v>
       </c>
       <c r="V3" s="3" cm="1">
         <f t="array" aca="1" ref="V3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>148312.60509733259</v>
+        <v>148837.495247938</v>
       </c>
       <c r="W3" s="3" cm="1">
         <f t="array" aca="1" ref="W3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>145367.88238800399</v>
+        <v>144931.95666970458</v>
       </c>
       <c r="X3" s="3" cm="1">
         <f t="array" aca="1" ref="X3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>147707.6469576518</v>
+        <v>144286.9645354861</v>
       </c>
       <c r="Y3" s="3" cm="1">
         <f t="array" aca="1" ref="Y3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>150799.16098028529</v>
+        <v>145105.43731270128</v>
       </c>
       <c r="Z3" s="3" cm="1">
         <f t="array" aca="1" ref="Z3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>155176.21104974049</v>
+        <v>146653.4184348257</v>
       </c>
       <c r="AA3" s="3" cm="1">
         <f t="array" aca="1" ref="AA3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>160861.03827409388</v>
+        <v>148917.56323701338</v>
       </c>
       <c r="AB3" s="3" cm="1">
         <f t="array" aca="1" ref="AB3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>167884.78020465258</v>
+        <v>151893.42349764908</v>
       </c>
       <c r="AC3" s="3" cm="1">
         <f t="array" aca="1" ref="AC3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>175477.89450196968</v>
+        <v>154918.21419605307</v>
       </c>
       <c r="AD3" s="3" cm="1">
         <f t="array" aca="1" ref="AD3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>183960.65312234679</v>
+        <v>158245.48396429748</v>
       </c>
       <c r="AE3" s="3" cm="1">
         <f t="array" aca="1" ref="AE3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>193519.88137362647</v>
+        <v>161981.99012114949</v>
       </c>
       <c r="AF3" s="3" cm="1">
         <f t="array" aca="1" ref="AF3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>204226.75080165357</v>
+        <v>166154.42199630089</v>
       </c>
       <c r="AG3" s="3" cm="1">
         <f t="array" aca="1" ref="AG3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>229221.30805802427</v>
+        <v>175762.58068534889</v>
       </c>
       <c r="AH3" s="3" cm="1">
         <f t="array" aca="1" ref="AH3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>259064.42687507198</v>
+        <v>186900.92761006008</v>
       </c>
       <c r="AI3" s="3" cm="1">
         <f t="array" aca="1" ref="AI3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>332357.77443037007</v>
+        <v>192954.95722848337</v>
       </c>
       <c r="AJ3" s="3" cm="1">
         <f t="array" aca="1" ref="AJ3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>342584.2359239448</v>
+        <v>192954.95722848337</v>
       </c>
       <c r="AK3" s="3" cm="1">
         <f t="array" aca="1" ref="AK3" ca="1" xml:space="preserve"> INDIRECT(ADDRESS(ROW()-1, COLUMN()))*4.4482216153</f>
-        <v>342584.2359239448</v>
+        <v>192954.95722848337</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
@@ -14640,7 +13874,117 @@
         <v>191976.3484731174</v>
       </c>
     </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>131440.5005104997</v>
+      </c>
+      <c r="C9">
+        <v>123571.59647303399</v>
+      </c>
+      <c r="D9">
+        <v>118651.86336651219</v>
+      </c>
+      <c r="E9">
+        <v>116258.72013748079</v>
+      </c>
+      <c r="F9">
+        <v>115902.86240825678</v>
+      </c>
+      <c r="G9">
+        <v>116058.55016479229</v>
+      </c>
+      <c r="H9">
+        <v>116694.6458557802</v>
+      </c>
+      <c r="I9">
+        <v>117780.01192991339</v>
+      </c>
+      <c r="J9">
+        <v>118785.31001497118</v>
+      </c>
+      <c r="K9">
+        <v>119879.57253233499</v>
+      </c>
+      <c r="L9">
+        <v>121133.97102784959</v>
+      </c>
+      <c r="M9">
+        <v>122535.16083666909</v>
+      </c>
+      <c r="N9">
+        <v>125635.57130253319</v>
+      </c>
+      <c r="O9">
+        <v>128758.2228764738</v>
+      </c>
+      <c r="P9">
+        <v>130159.41268529328</v>
+      </c>
+      <c r="Q9">
+        <v>130159.41268529328</v>
+      </c>
+      <c r="R9">
+        <v>130159.41268529328</v>
+      </c>
+    </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10">
+        <v>156372.7826642562</v>
+      </c>
+      <c r="C10">
+        <v>148837.495247938</v>
+      </c>
+      <c r="D10">
+        <v>144931.95666970458</v>
+      </c>
+      <c r="E10">
+        <v>144286.9645354861</v>
+      </c>
+      <c r="F10">
+        <v>145105.43731270128</v>
+      </c>
+      <c r="G10">
+        <v>146653.4184348257</v>
+      </c>
+      <c r="H10">
+        <v>148917.56323701338</v>
+      </c>
+      <c r="I10">
+        <v>151893.42349764908</v>
+      </c>
+      <c r="J10">
+        <v>154918.21419605307</v>
+      </c>
+      <c r="K10">
+        <v>158245.48396429748</v>
+      </c>
+      <c r="L10">
+        <v>161981.99012114949</v>
+      </c>
+      <c r="M10">
+        <v>166154.42199630089</v>
+      </c>
+      <c r="N10">
+        <v>175762.58068534889</v>
+      </c>
+      <c r="O10">
+        <v>186900.92761006008</v>
+      </c>
+      <c r="P10">
+        <v>192954.95722848337</v>
+      </c>
+      <c r="Q10">
+        <v>192954.95722848337</v>
+      </c>
+      <c r="R10">
+        <v>192954.95722848337</v>
+      </c>
       <c r="T10" t="s">
         <v>36</v>
       </c>
@@ -14800,6 +14144,330 @@
       </c>
       <c r="AK12">
         <v>342584.2359239448</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="T14" t="s">
+        <v>45</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0.2</v>
+      </c>
+      <c r="W14">
+        <v>0.4</v>
+      </c>
+      <c r="X14">
+        <v>0.6</v>
+      </c>
+      <c r="Y14">
+        <v>0.7</v>
+      </c>
+      <c r="Z14">
+        <v>0.8</v>
+      </c>
+      <c r="AA14">
+        <v>0.9</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AD14">
+        <v>1.2</v>
+      </c>
+      <c r="AE14">
+        <v>1.3</v>
+      </c>
+      <c r="AF14">
+        <v>1.4</v>
+      </c>
+      <c r="AG14">
+        <v>1.6</v>
+      </c>
+      <c r="AH14">
+        <v>1.8</v>
+      </c>
+      <c r="AI14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AJ14">
+        <v>2.5</v>
+      </c>
+      <c r="AK14">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="U15">
+        <v>29549</v>
+      </c>
+      <c r="V15">
+        <v>27780</v>
+      </c>
+      <c r="W15">
+        <v>26674</v>
+      </c>
+      <c r="X15">
+        <v>26136</v>
+      </c>
+      <c r="Y15">
+        <v>26056</v>
+      </c>
+      <c r="Z15">
+        <v>26091</v>
+      </c>
+      <c r="AA15">
+        <v>26234</v>
+      </c>
+      <c r="AB15">
+        <v>26478</v>
+      </c>
+      <c r="AC15">
+        <v>26704</v>
+      </c>
+      <c r="AD15">
+        <v>26950</v>
+      </c>
+      <c r="AE15">
+        <v>27232</v>
+      </c>
+      <c r="AF15">
+        <v>27547</v>
+      </c>
+      <c r="AG15">
+        <v>28244</v>
+      </c>
+      <c r="AH15">
+        <v>28946</v>
+      </c>
+      <c r="AI15">
+        <v>29261</v>
+      </c>
+      <c r="AJ15">
+        <v>29261</v>
+      </c>
+      <c r="AK15">
+        <v>29261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="U16">
+        <v>131440.5005104997</v>
+      </c>
+      <c r="V16">
+        <v>123571.59647303399</v>
+      </c>
+      <c r="W16">
+        <v>118651.86336651219</v>
+      </c>
+      <c r="X16">
+        <v>116258.72013748079</v>
+      </c>
+      <c r="Y16">
+        <v>115902.86240825678</v>
+      </c>
+      <c r="Z16">
+        <v>116058.55016479229</v>
+      </c>
+      <c r="AA16">
+        <v>116694.6458557802</v>
+      </c>
+      <c r="AB16">
+        <v>117780.01192991339</v>
+      </c>
+      <c r="AC16">
+        <v>118785.31001497118</v>
+      </c>
+      <c r="AD16">
+        <v>119879.57253233499</v>
+      </c>
+      <c r="AE16">
+        <v>121133.97102784959</v>
+      </c>
+      <c r="AF16">
+        <v>122535.16083666909</v>
+      </c>
+      <c r="AG16">
+        <v>125635.57130253319</v>
+      </c>
+      <c r="AH16">
+        <v>128758.2228764738</v>
+      </c>
+      <c r="AI16">
+        <v>130159.41268529328</v>
+      </c>
+      <c r="AJ16">
+        <v>130159.41268529328</v>
+      </c>
+      <c r="AK16">
+        <v>130159.41268529328</v>
+      </c>
+    </row>
+    <row r="18" spans="20:37" x14ac:dyDescent="0.2">
+      <c r="T18" t="s">
+        <v>46</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0.2</v>
+      </c>
+      <c r="W18">
+        <v>0.4</v>
+      </c>
+      <c r="X18">
+        <v>0.6</v>
+      </c>
+      <c r="Y18">
+        <v>0.7</v>
+      </c>
+      <c r="Z18">
+        <v>0.8</v>
+      </c>
+      <c r="AA18">
+        <v>0.9</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AD18">
+        <v>1.2</v>
+      </c>
+      <c r="AE18">
+        <v>1.3</v>
+      </c>
+      <c r="AF18">
+        <v>1.4</v>
+      </c>
+      <c r="AG18">
+        <v>1.6</v>
+      </c>
+      <c r="AH18">
+        <v>1.8</v>
+      </c>
+      <c r="AI18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AJ18">
+        <v>2.5</v>
+      </c>
+      <c r="AK18">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="19" spans="20:37" x14ac:dyDescent="0.2">
+      <c r="U19">
+        <v>35154</v>
+      </c>
+      <c r="V19">
+        <v>33460</v>
+      </c>
+      <c r="W19">
+        <v>32582</v>
+      </c>
+      <c r="X19">
+        <v>32437</v>
+      </c>
+      <c r="Y19">
+        <v>32621</v>
+      </c>
+      <c r="Z19">
+        <v>32969</v>
+      </c>
+      <c r="AA19">
+        <v>33478</v>
+      </c>
+      <c r="AB19">
+        <v>34147</v>
+      </c>
+      <c r="AC19">
+        <v>34827</v>
+      </c>
+      <c r="AD19">
+        <v>35575</v>
+      </c>
+      <c r="AE19">
+        <v>36415</v>
+      </c>
+      <c r="AF19">
+        <v>37353</v>
+      </c>
+      <c r="AG19">
+        <v>39513</v>
+      </c>
+      <c r="AH19">
+        <v>42017</v>
+      </c>
+      <c r="AI19">
+        <v>43378</v>
+      </c>
+      <c r="AJ19">
+        <v>43378</v>
+      </c>
+      <c r="AK19">
+        <v>43378</v>
+      </c>
+    </row>
+    <row r="20" spans="20:37" x14ac:dyDescent="0.2">
+      <c r="U20">
+        <v>156372.7826642562</v>
+      </c>
+      <c r="V20">
+        <v>148837.495247938</v>
+      </c>
+      <c r="W20">
+        <v>144931.95666970458</v>
+      </c>
+      <c r="X20">
+        <v>144286.9645354861</v>
+      </c>
+      <c r="Y20">
+        <v>145105.43731270128</v>
+      </c>
+      <c r="Z20">
+        <v>146653.4184348257</v>
+      </c>
+      <c r="AA20">
+        <v>148917.56323701338</v>
+      </c>
+      <c r="AB20">
+        <v>151893.42349764908</v>
+      </c>
+      <c r="AC20">
+        <v>154918.21419605307</v>
+      </c>
+      <c r="AD20">
+        <v>158245.48396429748</v>
+      </c>
+      <c r="AE20">
+        <v>161981.99012114949</v>
+      </c>
+      <c r="AF20">
+        <v>166154.42199630089</v>
+      </c>
+      <c r="AG20">
+        <v>175762.58068534889</v>
+      </c>
+      <c r="AH20">
+        <v>186900.92761006008</v>
+      </c>
+      <c r="AI20">
+        <v>192954.95722848337</v>
+      </c>
+      <c r="AJ20">
+        <v>192954.95722848337</v>
+      </c>
+      <c r="AK20">
+        <v>192954.95722848337</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>